<commit_message>
large commit of various bits
</commit_message>
<xml_diff>
--- a/Figures/SD_sum_W.xlsx
+++ b/Figures/SD_sum_W.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="SD_sum_W" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Estimate</t>
   </si>
@@ -122,6 +122,21 @@
   </si>
   <si>
     <t>R2=0.12</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>Standard error</t>
+  </si>
+  <si>
+    <t>T value</t>
   </si>
 </sst>
 </file>
@@ -955,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1328,6 +1343,23 @@
         <v>-1.19098195099136</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
@@ -1360,7 +1392,7 @@
         <v>16.950695276313869</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="C29:E33" si="0">C3</f>
+        <f t="shared" ref="D29:E33" si="0">C3</f>
         <v>1.0933818172896199</v>
       </c>
       <c r="E29">
@@ -1376,7 +1408,7 @@
         <v>1984</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:C44" si="1">$B$2+B4</f>
+        <f t="shared" ref="C30:C43" si="1">$B$2+B4</f>
         <v>15.997618875566538</v>
       </c>
       <c r="D30">
@@ -1676,7 +1708,7 @@
         <v>2014</v>
       </c>
       <c r="C45">
-        <f t="shared" ref="C45:D47" si="13">$B$2+B24</f>
+        <f t="shared" ref="C45:C47" si="13">$B$2+B24</f>
         <v>19.70459169516737</v>
       </c>
       <c r="D45">

</xml_diff>